<commit_message>
Nouvelle mise à jour
</commit_message>
<xml_diff>
--- a/inputcons/BD.xlsx
+++ b/inputcons/BD.xlsx
@@ -64,13 +64,13 @@
     <t>Quantité Relative</t>
   </si>
   <si>
-    <t>Drink</t>
-  </si>
-  <si>
-    <t>Eat</t>
-  </si>
-  <si>
-    <t>Smoke</t>
+    <t>DRINK</t>
+  </si>
+  <si>
+    <t>EAT</t>
+  </si>
+  <si>
+    <t>SMOKE</t>
   </si>
   <si>
     <t>SOFTS</t>

</xml_diff>

<commit_message>
Le 29 août 2023
</commit_message>
<xml_diff>
--- a/inputcons/BD.xlsx
+++ b/inputcons/BD.xlsx
@@ -64,13 +64,13 @@
     <t>Quantité Relative</t>
   </si>
   <si>
-    <t>Drink</t>
-  </si>
-  <si>
-    <t>Eat</t>
-  </si>
-  <si>
-    <t>Smoke</t>
+    <t>DRINK</t>
+  </si>
+  <si>
+    <t>EAT</t>
+  </si>
+  <si>
+    <t>SMOKE</t>
   </si>
   <si>
     <t>SOFTS</t>

</xml_diff>